<commit_message>
Initial commit: Add project files
</commit_message>
<xml_diff>
--- a/Input/input_data.xlsx
+++ b/Input/input_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\US81896\PycharmProjects\pythonProject1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{FAD1E3E0-D7F4-4645-BFB4-923D303F7E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A25C7CE-1225-4E00-B5A7-3A56C3D86BA5}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{FAD1E3E0-D7F4-4645-BFB4-923D303F7E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4074B8B6-6518-471E-AA3E-01413C428173}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="124">
   <si>
     <t>Subtask ID</t>
   </si>
@@ -95,6 +95,93 @@
     <t>Manage Transmission Configurations</t>
   </si>
   <si>
+    <t>Bills Receivable Config</t>
+  </si>
+  <si>
+    <t>File Directory</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>Append To File (Y/N)</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtask ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processs Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requires the Configuration Name required, Required the config In which the Column needs to be updated </t>
+  </si>
+  <si>
+    <t>Manage Administrative Profile Values</t>
+  </si>
+  <si>
+    <t>Just Required the Value1 for it Which will change the Banner name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESS Job Submission </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Value Required </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manage Disbursement System Option </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Put the Value of email needs to be changed </t>
+  </si>
+  <si>
+    <t>Manage Supplier Notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run GL Process </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send the Value for  need to pass the value for it </t>
+  </si>
+  <si>
+    <t>Disable Printer</t>
+  </si>
+  <si>
+    <t>Disable Notification in BPM worklist</t>
+  </si>
+  <si>
+    <t>Manage Journal Approvals</t>
+  </si>
+  <si>
+    <t>Security Console</t>
+  </si>
+  <si>
+    <t>Just Required the User Name</t>
+  </si>
+  <si>
+    <t>Manage Payment Process Profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just Required the One Value for it </t>
+  </si>
+  <si>
+    <t>Manage Receivables System Options</t>
+  </si>
+  <si>
+    <t>Sni</t>
+  </si>
+  <si>
     <t>SDD - Acknowledgement</t>
   </si>
   <si>
@@ -110,72 +197,6 @@
     <t>dmsmpmspdmpsmdp</t>
   </si>
   <si>
-    <t xml:space="preserve">Subtask ID </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processs Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requires the Configuration Name required, Required the config In which the Column needs to be updated </t>
-  </si>
-  <si>
-    <t>Manage Administrative Profile Values</t>
-  </si>
-  <si>
-    <t>Just Required the Value1 for it Which will change the Banner name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESS Job Submission </t>
-  </si>
-  <si>
-    <t xml:space="preserve">No Value Required </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manage Disbursement System Option </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Put the Value of email needs to be changed </t>
-  </si>
-  <si>
-    <t>Manage Supplier Notification</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Run GL Process </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Send the Value for  need to pass the value for it </t>
-  </si>
-  <si>
-    <t>Disable Printer</t>
-  </si>
-  <si>
-    <t>Disable Notification in BPM worklist</t>
-  </si>
-  <si>
-    <t>Manage Journal Approvals</t>
-  </si>
-  <si>
-    <t>Security Console</t>
-  </si>
-  <si>
-    <t>Just Required the User Name</t>
-  </si>
-  <si>
-    <t>Manage Payment Process Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just Required the One Value for it </t>
-  </si>
-  <si>
-    <t>Manage Receivables System Options</t>
-  </si>
-  <si>
-    <t>Sni</t>
-  </si>
-  <si>
     <t>Manage Administrator Profile Values</t>
   </si>
   <si>
@@ -252,27 +273,6 @@
   </si>
   <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>Bills Receivable Config</t>
-  </si>
-  <si>
-    <t>File Directory</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>File Name</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>Append To File (Y/N)</t>
-  </si>
-  <si>
-    <t>test3</t>
   </si>
   <si>
     <t>testing is goijng on of P2T automation</t>
@@ -828,7 +828,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -903,8 +903,12 @@
       <c r="G2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
@@ -919,7 +923,7 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -931,13 +935,13 @@
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -948,7 +952,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -956,10 +960,10 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -967,10 +971,10 @@
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -978,10 +982,10 @@
         <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -989,10 +993,10 @@
         <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -1000,10 +1004,10 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -1011,10 +1015,10 @@
         <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1022,10 +1026,10 @@
         <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -1033,10 +1037,10 @@
         <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -1044,10 +1048,10 @@
         <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -1055,10 +1059,10 @@
         <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -1066,15 +1070,15 @@
         <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:4">
       <c r="D17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1086,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9868C259-FF60-4EA9-9DDA-810F97FA19C4}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1110,19 +1114,19 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1134,16 +1138,16 @@
         <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
@@ -1156,20 +1160,20 @@
         <v>103</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1181,10 +1185,10 @@
         <v>104</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1200,21 +1204,21 @@
         <v>105</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1225,10 +1229,10 @@
         <v>106</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1247,31 +1251,31 @@
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1282,19 +1286,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1309,25 +1313,25 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1340,19 +1344,19 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1364,13 +1368,13 @@
         <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
         <v>72</v>
@@ -1381,21 +1385,21 @@
         <v>103</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1412,17 +1416,17 @@
         <v>104</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>75</v>
@@ -1440,22 +1444,22 @@
         <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>76</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>77</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>78</v>
@@ -1471,16 +1475,16 @@
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>80</v>
@@ -1495,13 +1499,13 @@
         <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
         <v>81</v>
@@ -1520,7 +1524,7 @@
         <v>106</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>83</v>
@@ -1551,7 +1555,7 @@
         <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1575,7 +1579,7 @@
         <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>92</v>
@@ -1594,7 +1598,7 @@
         <v>111</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
         <v>93</v>
@@ -1605,7 +1609,7 @@
         <v>111</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
         <v>94</v>
@@ -1616,7 +1620,7 @@
         <v>111</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
         <v>95</v>
@@ -1627,13 +1631,13 @@
         <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D59" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E59" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F59" t="s">
         <v>81</v>
@@ -1652,7 +1656,7 @@
         <v>106</v>
       </c>
       <c r="C61" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>83</v>
@@ -1683,7 +1687,7 @@
         <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -1707,7 +1711,7 @@
         <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>92</v>
@@ -1911,13 +1915,13 @@
         <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>119</v>
@@ -1933,7 +1937,7 @@
         <v>105</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1981,7 +1985,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1998,7 +2002,7 @@
         <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2015,7 +2019,7 @@
         <v>109</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -2032,7 +2036,7 @@
         <v>110</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>92</v>
@@ -2051,7 +2055,7 @@
         <v>111</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>93</v>
@@ -2070,7 +2074,7 @@
         <v>111</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>94</v>
@@ -2089,7 +2093,7 @@
         <v>111</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>95</v>
@@ -2108,7 +2112,7 @@
         <v>112</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>121</v>
@@ -2127,7 +2131,7 @@
         <v>112</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>122</v>
@@ -2146,13 +2150,13 @@
         <v>102</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>123</v>
@@ -2189,13 +2193,13 @@
         <v>118</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>119</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>119</v>
@@ -2211,7 +2215,7 @@
         <v>105</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2259,7 +2263,7 @@
         <v>107</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2276,7 +2280,7 @@
         <v>108</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2293,7 +2297,7 @@
         <v>109</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2310,7 +2314,7 @@
         <v>110</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>92</v>
@@ -2329,7 +2333,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>93</v>
@@ -2348,7 +2352,7 @@
         <v>111</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>94</v>
@@ -2367,7 +2371,7 @@
         <v>111</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>95</v>
@@ -2386,7 +2390,7 @@
         <v>112</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>121</v>
@@ -2405,7 +2409,7 @@
         <v>112</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>122</v>
@@ -2431,12 +2435,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C5422AC91CF8E947A984DCE6015D273C" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f32ea5a1cd566b128aa76ed9b4b5df4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fb5a1ccf-a65f-4902-b56f-6f19daef6027" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74d29ba8d220cbabd832619bca9f6aa8" ns2:_="">
     <xsd:import namespace="fb5a1ccf-a65f-4902-b56f-6f19daef6027"/>
@@ -2580,6 +2578,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2590,11 +2594,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA43252-5667-4C8C-9731-F5D0DBAA4343}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E22E01A-42DF-4875-95E2-B6A285A4A10C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E22E01A-42DF-4875-95E2-B6A285A4A10C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA43252-5667-4C8C-9731-F5D0DBAA4343}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>